<commit_message>
adding final demo data to week 8 lab
</commit_message>
<xml_diff>
--- a/08-motion-adaptation/motion-adaptation/motion-adaptation.xlsx
+++ b/08-motion-adaptation/motion-adaptation/motion-adaptation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://indiana-my.sharepoint.com/personal/kbonnen_iu_edu/Documents/Courses/V768-Measuring-Perception/V768-Psychophysics-labs/08-motion-adaptation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://indiana-my.sharepoint.com/personal/kbonnen_iu_edu/Documents/Courses/V768-Measuring-Perception/V768-Psychophysics-labs/08-motion-adaptation/motion-adaptation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{DBB62FA1-4837-F44A-8B28-60C9FD47805A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{654C51C3-D796-9845-A0B0-5ACE3A795A40}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="8_{DBB62FA1-4837-F44A-8B28-60C9FD47805A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EDC8AA0B-5A0A-4045-9C7F-B5E493335BDB}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -517,7 +517,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
+      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -534,7 +534,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
+      <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
@@ -542,7 +542,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
+      <c r="A3">
         <v>0.5</v>
       </c>
       <c r="B3">
@@ -550,39 +550,39 @@
       </c>
     </row>
     <row r="4" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>0.25</v>
+      <c r="A4">
+        <v>0.4</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
-        <v>0.125</v>
+      <c r="A5">
+        <v>0.3</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
-        <v>6.25E-2</v>
+      <c r="A6">
+        <v>0.2</v>
       </c>
       <c r="B6">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
-        <v>3.125E-2</v>
+      <c r="A7">
+        <v>0.1</v>
       </c>
       <c r="B7">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
+      <c r="A8">
         <v>0</v>
       </c>
       <c r="B8">
@@ -590,7 +590,7 @@
       </c>
     </row>
     <row r="9" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
+      <c r="A9">
         <v>1</v>
       </c>
       <c r="B9">
@@ -598,7 +598,7 @@
       </c>
     </row>
     <row r="10" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
+      <c r="A10">
         <v>0.5</v>
       </c>
       <c r="B10">
@@ -606,39 +606,39 @@
       </c>
     </row>
     <row r="11" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
-        <v>0.25</v>
+      <c r="A11">
+        <v>0.4</v>
       </c>
       <c r="B11">
         <v>180</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="1">
-        <v>0.125</v>
+      <c r="A12">
+        <v>0.3</v>
       </c>
       <c r="B12">
         <v>180</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="1">
-        <v>6.25E-2</v>
+      <c r="A13">
+        <v>0.2</v>
       </c>
       <c r="B13">
         <v>180</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="1">
-        <v>3.125E-2</v>
+      <c r="A14">
+        <v>0.1</v>
       </c>
       <c r="B14">
         <v>180</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="1">
+      <c r="A15">
         <v>0</v>
       </c>
       <c r="B15">
@@ -667,12 +667,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B9F5CAB0486A994CA2C3B13E059EF2AE" ma:contentTypeVersion="0" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="8645ec4a60d0c8c7009d2d6675847a91">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="636d7205651659ec4fcda0bcbde9384b">
     <xsd:element name="properties">
@@ -786,6 +780,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3744155D-8FAB-4E67-B5E0-C7FDBFB3715D}">
   <ds:schemaRefs>
@@ -795,21 +795,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3725960-8A89-4E70-9C40-340E0EDB6403}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EFF1C174-6AC6-4774-A736-3226A12360E4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -823,4 +808,19 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3725960-8A89-4E70-9C40-340E0EDB6403}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>